<commit_message>
minor changes in FFQ sample data
</commit_message>
<xml_diff>
--- a/data/sample_ffq.xlsx
+++ b/data/sample_ffq.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="328">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -719,7 +719,7 @@
     <t xml:space="preserve">ID_00117</t>
   </si>
   <si>
-    <t xml:space="preserve">Cauliflower...123</t>
+    <t xml:space="preserve">Cauliflower</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00118</t>
@@ -833,373 +833,169 @@
     <t xml:space="preserve">ID_00136</t>
   </si>
   <si>
-    <t xml:space="preserve">What type of milk did you most often use? Select one only</t>
+    <t xml:space="preserve">Fish and fish products</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00137</t>
   </si>
   <si>
-    <t xml:space="preserve">Approximately, how much milk did you drink each day, including milk with tea, coffee, cereals etc?</t>
+    <t xml:space="preserve">Meat, meat products and meat dishes (including bacon, ham and chicken)</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00138</t>
   </si>
   <si>
-    <t xml:space="preserve">What kind of fat did you most often use for frying, roasting, grilling etc? Select one only</t>
+    <t xml:space="preserve">Asparagus</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00139</t>
   </si>
   <si>
-    <t xml:space="preserve">How often did you eat food that was fried at home? Select one only</t>
+    <t xml:space="preserve">Artichoke</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00140</t>
   </si>
   <si>
-    <t xml:space="preserve">How often did you eat fried food away from home? Select one only</t>
+    <t xml:space="preserve">Beansprouts...171</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00141</t>
   </si>
   <si>
-    <t xml:space="preserve">How often did you add salt to food while cooking? Select one only</t>
+    <t xml:space="preserve">Beetroot</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00142</t>
   </si>
   <si>
-    <t xml:space="preserve">How often did you add salt to any food at the table? Select one only</t>
+    <t xml:space="preserve">Broad beans</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00143</t>
   </si>
   <si>
-    <t xml:space="preserve">1. No</t>
+    <t xml:space="preserve">Brocoli</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00144</t>
   </si>
   <si>
-    <t xml:space="preserve">2. Yes, because of a medical condition/allergy</t>
+    <t xml:space="preserve">Brussel sprouts</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00145</t>
   </si>
   <si>
-    <t xml:space="preserve">3. Yes, to lose weight</t>
+    <t xml:space="preserve">Cauliflower...176</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00146</t>
   </si>
   <si>
-    <t xml:space="preserve">4. Yes, because of personal beliefs (religion, vegetarian)</t>
+    <t xml:space="preserve">Cabbage...177</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00147</t>
   </si>
   <si>
-    <t xml:space="preserve">5. Yes, other</t>
+    <t xml:space="preserve">Chick peas</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00148</t>
   </si>
   <si>
-    <t xml:space="preserve">Over the last 6 months, how often have you eaten organic foods? Select one only</t>
+    <t xml:space="preserve">courgette</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00149</t>
   </si>
   <si>
-    <t xml:space="preserve">a. Vitamins (e.g. multivitamins, vitamin B, vitamin C, folic acid)</t>
+    <t xml:space="preserve">Curly kale</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00150</t>
   </si>
   <si>
-    <t xml:space="preserve">If yes, what type and when :...156</t>
+    <t xml:space="preserve">Green beans</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00151</t>
   </si>
   <si>
-    <t xml:space="preserve">b. Minerals (e.g. iron, calcium, zinc, magnesium)</t>
+    <t xml:space="preserve">Leeks...182</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00152</t>
   </si>
   <si>
-    <t xml:space="preserve">If yes, what type and when :...158</t>
+    <t xml:space="preserve">Lentils</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00153</t>
   </si>
   <si>
-    <t xml:space="preserve">c. Fish oils (e.g. cod liver oil, omega-3)</t>
+    <t xml:space="preserve">Lettuce</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00154</t>
   </si>
   <si>
-    <t xml:space="preserve">If yes, what type and when :...160</t>
+    <t xml:space="preserve">Mixed Veg Frozen</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00155</t>
   </si>
   <si>
-    <t xml:space="preserve">d. Other food supplements (e.g. oil of evening primose, starflower oil, royal jelly, ginseng)</t>
+    <t xml:space="preserve">Mixed Veg Canned</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00156</t>
   </si>
   <si>
-    <t xml:space="preserve">If yes, what type and when :...162</t>
+    <t xml:space="preserve">Parsnips</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00157</t>
   </si>
   <si>
-    <t xml:space="preserve">Vegetables (not including potatoes)</t>
+    <t xml:space="preserve">Peas...188</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00158</t>
   </si>
   <si>
-    <t xml:space="preserve">Salads</t>
+    <t xml:space="preserve">Red Kidney Beans</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00159</t>
   </si>
   <si>
-    <t xml:space="preserve">Fruit and fruit products (not including fruit juice)</t>
+    <t xml:space="preserve">Runner Beans</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00160</t>
   </si>
   <si>
-    <t xml:space="preserve">Fish and fish products</t>
+    <t xml:space="preserve">Spinach fresh</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00161</t>
   </si>
   <si>
-    <t xml:space="preserve">Meat, meat products and meat dishes (including bacon, ham and chicken)</t>
+    <t xml:space="preserve">Spinach frozen</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00162</t>
   </si>
   <si>
-    <t xml:space="preserve">How often do you eat fruit or vegetables from a garden or allotment?</t>
+    <t xml:space="preserve">Sweetcorn fresh</t>
   </si>
   <si>
     <t xml:space="preserve">ID_00163</t>
   </si>
   <si>
-    <t xml:space="preserve">Asparagus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00164</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artichoke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00165</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beansprouts...171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beetroot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00167</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Broad beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brocoli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00169</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brussel sprouts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cauliflower...176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cabbage...177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chick peas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00173</t>
-  </si>
-  <si>
-    <t xml:space="preserve">courgette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curly kale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leeks...182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lentils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lettuce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mixed Veg Frozen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mixed Veg Canned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parsnips</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peas...188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red Kidney Beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runner Beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00185</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spinach fresh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spinach frozen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweetcorn fresh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00188</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sweetcorn canned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00189</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not eaten...195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1...196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00191</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2...197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00192</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3...198</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not eaten...199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00194</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1...200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2...201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3...202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_00197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sexe </t>
   </si>
 </sst>
 </file>
@@ -2843,278 +2639,6 @@
         <v>327</v>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" t="s">
-        <v>328</v>
-      </c>
-      <c r="B165" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="s">
-        <v>330</v>
-      </c>
-      <c r="B166" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="s">
-        <v>332</v>
-      </c>
-      <c r="B167" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="s">
-        <v>334</v>
-      </c>
-      <c r="B168" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="s">
-        <v>336</v>
-      </c>
-      <c r="B169" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="s">
-        <v>338</v>
-      </c>
-      <c r="B170" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="s">
-        <v>340</v>
-      </c>
-      <c r="B171" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="s">
-        <v>342</v>
-      </c>
-      <c r="B172" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="s">
-        <v>344</v>
-      </c>
-      <c r="B173" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="s">
-        <v>346</v>
-      </c>
-      <c r="B174" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="s">
-        <v>348</v>
-      </c>
-      <c r="B175" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="s">
-        <v>350</v>
-      </c>
-      <c r="B176" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="s">
-        <v>352</v>
-      </c>
-      <c r="B177" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="s">
-        <v>354</v>
-      </c>
-      <c r="B178" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="s">
-        <v>356</v>
-      </c>
-      <c r="B179" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="s">
-        <v>358</v>
-      </c>
-      <c r="B180" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="s">
-        <v>360</v>
-      </c>
-      <c r="B181" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="s">
-        <v>362</v>
-      </c>
-      <c r="B182" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="s">
-        <v>364</v>
-      </c>
-      <c r="B183" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="s">
-        <v>366</v>
-      </c>
-      <c r="B184" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="s">
-        <v>368</v>
-      </c>
-      <c r="B185" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="s">
-        <v>370</v>
-      </c>
-      <c r="B186" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="s">
-        <v>372</v>
-      </c>
-      <c r="B187" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="s">
-        <v>374</v>
-      </c>
-      <c r="B188" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="s">
-        <v>376</v>
-      </c>
-      <c r="B189" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="s">
-        <v>378</v>
-      </c>
-      <c r="B190" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="s">
-        <v>380</v>
-      </c>
-      <c r="B191" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="s">
-        <v>382</v>
-      </c>
-      <c r="B192" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="s">
-        <v>384</v>
-      </c>
-      <c r="B193" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="s">
-        <v>386</v>
-      </c>
-      <c r="B194" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="s">
-        <v>388</v>
-      </c>
-      <c r="B195" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="s">
-        <v>390</v>
-      </c>
-      <c r="B196" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="s">
-        <v>392</v>
-      </c>
-      <c r="B197" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="s">
-        <v>394</v>
-      </c>
-      <c r="B198" t="s">
-        <v>395</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>